<commit_message>
done with bsiks proof reading
</commit_message>
<xml_diff>
--- a/tukey_kramer.xlsx
+++ b/tukey_kramer.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,73 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\TAMU\Spring_2023\final_proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A34C6771-D5C0-4008-A659-88857864D621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F77C895-3C50-408A-9DB2-11F7ED5FBD97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tukey_kramer" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">tukey_kramer!$C$12:$C$20</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">tukey_kramer!$D$12:$D$20</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">tukey_kramer!$C$12:$C$14</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">tukey_kramer!$C$12:$C$17</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">tukey_kramer!$C$12:$C$20</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">tukey_kramer!$C$12:$C$29</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">tukey_kramer!$D$12:$D$14</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">tukey_kramer!$D$12:$D$17</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">tukey_kramer!$D$12:$D$20</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">tukey_kramer!$D$12:$D$29</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">tukey_kramer!$C$12:$C$19</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">tukey_kramer!$C$12:$C$20</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">tukey_kramer!$C$12:$C$14</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">tukey_kramer!$C$20</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">tukey_kramer!$D$12</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">tukey_kramer!$D$12:$D$19</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">tukey_kramer!$D$12:$D$20</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">tukey_kramer!$H$22</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">tukey_kramer!$C$12:$C$20</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">tukey_kramer!$D$12:$D$20</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">tukey_kramer!$C$12:$C$14</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">tukey_kramer!$C$12:$C$17</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">tukey_kramer!$C$12:$C$20</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">tukey_kramer!$C$12:$C$17</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">tukey_kramer!$C$12:$C$29</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">tukey_kramer!$D$12:$D$14</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">tukey_kramer!$D$12:$D$17</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">tukey_kramer!$D$12:$D$20</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">tukey_kramer!$D$12:$D$29</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">tukey_kramer!$C$12:$C$14</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">tukey_kramer!$C$12:$C$17</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">tukey_kramer!$C$12:$C$20</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">tukey_kramer!$C$12:$C$29</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">tukey_kramer!$D$12:$D$14</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">tukey_kramer!$C$12:$C$20</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">tukey_kramer!$D$12:$D$17</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">tukey_kramer!$D$12:$D$20</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">tukey_kramer!$D$12:$D$29</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">tukey_kramer!$C$12:$C$14</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">tukey_kramer!$C$12:$C$17</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">tukey_kramer!$C$12:$C$20</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">tukey_kramer!$C$12:$C$29</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">tukey_kramer!$D$12:$D$14</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">tukey_kramer!$D$12:$D$17</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">tukey_kramer!$D$12:$D$20</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">tukey_kramer!$C$12:$C$29</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">tukey_kramer!$D$12:$D$29</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">tukey_kramer!$C$12:$C$14</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">tukey_kramer!$C$12:$C$17</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">tukey_kramer!$C$12:$C$20</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">tukey_kramer!$C$12:$C$29</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">tukey_kramer!$D$12:$D$14</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">tukey_kramer!$D$12:$D$17</definedName>
-    <definedName name="_xlchart.v1.57" hidden="1">tukey_kramer!$D$12:$D$20</definedName>
-    <definedName name="_xlchart.v1.58" hidden="1">tukey_kramer!$D$12:$D$29</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">tukey_kramer!$D$12:$D$14</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">tukey_kramer!$D$12:$D$17</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">tukey_kramer!$D$12:$D$20</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">tukey_kramer!$D$12:$D$29</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">tukey_kramer!$C$12:$C$29</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">tukey_kramer!$D$12:$D$29</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -82,15 +25,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
-  <si>
-    <t>diff</t>
-  </si>
-  <si>
-    <t>lwr</t>
-  </si>
-  <si>
-    <t>upr</t>
-  </si>
   <si>
     <t>p adj</t>
   </si>
@@ -115,15 +49,25 @@
   <si>
     <t>Groups</t>
   </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>Lower</t>
+  </si>
+  <si>
+    <t>Upper</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,8 +202,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -439,8 +398,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -555,6 +526,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -600,10 +586,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -667,10 +658,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.30</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.34</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -773,29 +764,32 @@
         <cx:valScaling max="350" min="-250"/>
         <cx:title>
           <cx:tx>
-            <cx:rich>
-              <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr algn="ctr" rtl="0">
-                  <a:defRPr sz="1600" b="1">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1"/>
-                    </a:solidFill>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-                  </a:rPr>
-                  <a:t>Tukey Velocity Mean Difference</a:t>
-                </a:r>
-              </a:p>
-            </cx:rich>
+            <cx:txData>
+              <cx:v>Tukey Velocity Mean Difference</cx:v>
+            </cx:txData>
           </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1600" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:defRPr>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Tukey Velocity Mean Difference</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
         </cx:title>
         <cx:majorGridlines>
           <cx:spPr>
@@ -1440,8 +1434,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5166359" y="701992"/>
-              <a:ext cx="5579745" cy="4431983"/>
+              <a:off x="5170169" y="703897"/>
+              <a:ext cx="5574030" cy="4428173"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1770,143 +1764,142 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="2" max="4" width="10.44140625" customWidth="1"/>
+    <col min="5" max="5" width="6.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" s="5">
+        <v>-179.11823361823301</v>
+      </c>
+      <c r="C2" s="5">
+        <v>-198.55021512213801</v>
+      </c>
+      <c r="D2" s="5">
+        <v>-159.68625211432899</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B3" s="5">
+        <v>-151.26638176638201</v>
+      </c>
+      <c r="C3" s="5">
+        <v>-170.69836327028599</v>
+      </c>
+      <c r="D3" s="5">
+        <v>-131.834400262477</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B4" s="5">
+        <v>141.51139601139599</v>
+      </c>
+      <c r="C4" s="5">
+        <v>122.079414507492</v>
+      </c>
+      <c r="D4" s="5">
+        <v>160.94337751530099</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2">
-        <v>-179.11823361823301</v>
-      </c>
-      <c r="C2" s="1">
-        <v>-198.55021512213801</v>
-      </c>
-      <c r="D2" s="1">
-        <v>-159.68625211432899</v>
-      </c>
-      <c r="E2">
+      <c r="B5" s="5">
+        <v>27.851851851851698</v>
+      </c>
+      <c r="C5" s="5">
+        <v>8.6040639031125501</v>
+      </c>
+      <c r="D5" s="5">
+        <v>47.0996398005909</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1.48698812140247E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>320.62962962963002</v>
+      </c>
+      <c r="C6" s="5">
+        <v>301.38184168088998</v>
+      </c>
+      <c r="D6" s="5">
+        <v>339.87741757836898</v>
+      </c>
+      <c r="E6" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2">
-        <v>-151.26638176638201</v>
-      </c>
-      <c r="C3" s="1">
-        <v>-170.69836327028599</v>
-      </c>
-      <c r="D3" s="1">
-        <v>-131.834400262477</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2">
-        <v>141.51139601139599</v>
-      </c>
-      <c r="C4" s="1">
-        <v>122.079414507492</v>
-      </c>
-      <c r="D4" s="1">
-        <v>160.94337751530099</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2">
-        <v>27.851851851851698</v>
-      </c>
-      <c r="C5" s="1">
-        <v>8.6040639031125501</v>
-      </c>
-      <c r="D5" s="1">
-        <v>47.0996398005909</v>
-      </c>
-      <c r="E5">
-        <v>1.48698812140247E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2">
-        <v>320.62962962963002</v>
-      </c>
-      <c r="C6" s="1">
-        <v>301.38184168088998</v>
-      </c>
-      <c r="D6" s="1">
-        <v>339.87741757836898</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="B7" s="5">
         <v>292.777777777778</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="5">
         <v>273.52998982903898</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="5">
         <v>312.02556572651702</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2">
         <v>-179.11823361823301</v>
@@ -1914,7 +1907,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D13" s="1">
         <v>-198.55021512213801</v>
@@ -1922,7 +1915,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D14" s="1">
         <v>-159.68625211432899</v>
@@ -1930,7 +1923,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D15" s="2">
         <v>-151.26638176638201</v>
@@ -1938,7 +1931,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D16" s="1">
         <v>-170.69836327028599</v>
@@ -1946,7 +1939,7 @@
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D17" s="1">
         <v>-131.834400262477</v>
@@ -1954,7 +1947,7 @@
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D18" s="2">
         <v>141.51139601139599</v>
@@ -1962,7 +1955,7 @@
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D19" s="1">
         <v>122.079414507492</v>
@@ -1970,7 +1963,7 @@
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D20" s="1">
         <v>160.94337751530099</v>
@@ -1978,7 +1971,7 @@
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D21" s="2">
         <v>27.851851851851698</v>
@@ -1986,7 +1979,7 @@
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D22" s="1">
         <v>8.6040639031125501</v>
@@ -1994,7 +1987,7 @@
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D23" s="1">
         <v>47.0996398005909</v>
@@ -2002,7 +1995,7 @@
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D24" s="2">
         <v>320.62962962963002</v>
@@ -2010,7 +2003,7 @@
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D25" s="1">
         <v>301.38184168088998</v>
@@ -2018,7 +2011,7 @@
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D26" s="1">
         <v>339.87741757836898</v>
@@ -2026,7 +2019,7 @@
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D27" s="2">
         <v>292.777777777778</v>
@@ -2034,7 +2027,7 @@
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D28" s="1">
         <v>273.52998982903898</v>
@@ -2042,7 +2035,7 @@
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D29" s="1">
         <v>312.02556572651702</v>
@@ -2050,6 +2043,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>